<commit_message>
switching to openai 4o
</commit_message>
<xml_diff>
--- a/Book1 1.xlsx
+++ b/Book1 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TalAb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eladsoftwaresystems-my.sharepoint.com/personal/talab_elad_co_il/Documents/Desktop/Colmobil_POC/colmobil-chatbot-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B741C08E-1C71-489F-AFA1-57AC8621E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B741C08E-1C71-489F-AFA1-57AC8621E1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ADFB262-5059-4E1A-A292-76188790BEB4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD0C579A-840A-4C57-A2A4-D222709C2F4B}"/>
   </bookViews>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171052E1-CE14-464C-B376-E468AEA106A6}">
   <dimension ref="A1:AT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1037,7 +1037,7 @@
     <col min="3" max="3" width="14.625" customWidth="1"/>
     <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="5" width="12.125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="28.625" customWidth="1"/>
     <col min="7" max="7" width="129.875" customWidth="1"/>
     <col min="9" max="9" width="18.25" customWidth="1"/>
     <col min="42" max="42" width="16.25" customWidth="1"/>

</xml_diff>